<commit_message>
atualizacoes (nao incluir base)
atualizacoes (nao incluir base)
</commit_message>
<xml_diff>
--- a/datasets/exclusoes_julgamentais.xlsx
+++ b/datasets/exclusoes_julgamentais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielsaraivaleite/TCC/Codigo/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10ADF22-42BD-8244-B173-60D175943B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87E15B-7F5E-AB45-B180-9E98F2BF9881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="894">
   <si>
     <t>titulo</t>
   </si>
@@ -5012,6 +5012,366 @@
   <si>
     <t>dd9cc0cb1ce6135af9bd6563ac079199f733ae02e82a9bd6d60dfc98fcf4019c</t>
   </si>
+  <si>
+    <t>Inter recebe selo Pró-Ética - blog.inter.co</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiVWh0dHBzOi8vYmxvZy5pbnRlci5jby9pbnRlci1lLWRlc3RhcXVlLWVtLWludGVncmlkYWRlLWUtcmVjZWJlLXNlbG8tcHJvLWV0aWNhLWRhLWNndS_SAQA?oc=5</t>
+  </si>
+  <si>
+    <t>Blog.inter.co</t>
+  </si>
+  <si>
+    <t>banco inter</t>
+  </si>
+  <si>
+    <t>Banco Inter</t>
+  </si>
+  <si>
+    <t>BIDI4</t>
+  </si>
+  <si>
+    <t>00.416.968/0001-01</t>
+  </si>
+  <si>
+    <t>BANCO INTER S.A.</t>
+  </si>
+  <si>
+    <t>O Inter recebeu o selo Empresa Pró-Ética 2022-2023, maior reconhecimento à integridade e à ética no meio corporativo.
+A companhia é uma das 84 destacadas pela Controladoria Geral da União após uma avaliação rigorosa ao longo do ano. Uma das líderes em tecnologia para serviços financeiros, a empresa está sempre empenhada em manter os mais altos padrões éticos em todos os processos e produtos oferecidos para seus mais de 30 milhões de clientes.
+Quer saber mais sobre essa conquista? Então é ficar com a gente nesse post.</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) G (Governança).
+c) +1.0.
+d) Inter.
+e) Sim.
+f) O Inter foi reconhecido com o selo Empresa Pró-Ética 2022-2023 pela Controladoria Geral da União, destacando-se por sua integridade e ética corporativa.</t>
+  </si>
+  <si>
+    <t>795a9cabe77014dc24ad03edd84d41529e3c1df48cdae4f3e414b4d5a9dc7a5d</t>
+  </si>
+  <si>
+    <t>['ESG', 'G', 1.0, 'Inter', 'Sim', 'O Inter foi reconhecido com o selo Empresa Pró-Ética 2022-2023 pela Controladoria Geral da União, destacando-se por sua integridade e ética corporativa.']</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>O Inter foi reconhecido com o selo Empresa Pró-Ética 2022-2023 pela Controladoria Geral da União, destacando-se por sua integridade e ética corporativa.</t>
+  </si>
+  <si>
+    <t>Hapvida e NotreDame Intermédica apresentarão potenciais sinergias da fusão no dia 7 — Setor Saúde - Setor Saúde</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMibmh0dHBzOi8vc2V0b3JzYXVkZS5jb20uYnIvaGFwdmlkYS1lLW5vdHJlZGFtZS1pbnRlcm1lZGljYS1hcHJlc2VudGFyYW8tcG90ZW5jaWFpcy1zaW5lcmdpYXMtZGEtZnVzYW8tbm8tZGlhLTcv0gEA?oc=5</t>
+  </si>
+  <si>
+    <t>Setor saúde</t>
+  </si>
+  <si>
+    <t>notredame intermedica</t>
+  </si>
+  <si>
+    <t>A Hapvida e o Grupo NotreDame Intermédica (GNDI) realizarão um webcast (em português, com tradução simultânea para o inglês) para acionistas, analistas, investidores e o mercado em geral sobre as potenciais sinergias relacionadas à combinação/fusão entre Hapvida e GNDI. O CADE aprovou a fusão no início de janeiro.
+A atividade ocorre no dia 7 de fevereiro de 2022, segunda-feira, às 10h (horário de Brasília), 8h (horário de Nova York), com duração prevista de 1 hora.
+Representando a GNDI, estarão presentes Irlau Machado (CEO), Marcelo Moreira (CFO) e Glauco Desidério (Diretor de Relações com Investidores). Pela Hapvida, estarão presentes Jorge Pinheiro (CEO), Maurício Teixeira (CFO) e Guilherme Nahuz (Diretor de Relações com Investidores e ESG).
+Como assistir
+Para acompanhar é preciso acessar o site de Relações com Investidores (RI) das empresas:
+A apresentação que será utilizada no webcast poderá ser acessada pelo site de RI das Companhias cerca de 30 minutos antes do evento ou durante o próprio webcast.</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) G (Governança).
+c) 0.3 (A notícia tem um tom neutro, mas a menção de sinergias e a aprovação pelo CADE sugerem uma perspectiva positiva sob a ótica de governança).
+d) Hapvida e NotreDame Intermédica.
+e) Sim.
+f) A Hapvida e o Grupo NotreDame Intermédica realizarão um webcast para discutir as sinergias da fusão aprovada pelo CADE.</t>
+  </si>
+  <si>
+    <t>b6c13d0b123eaa967f1e49f8739f33c657d8269e617836def676966c2fe762df</t>
+  </si>
+  <si>
+    <t>['ESG', 'G', 0.3, 'Hapvida e NotreDame Intermédica', 'Sim', 'A Hapvida e o Grupo NotreDame Intermédica realizarão um webcast para discutir as sinergias da fusão aprovada pelo CADE.']</t>
+  </si>
+  <si>
+    <t>Hapvida e NotreDame Intermédica</t>
+  </si>
+  <si>
+    <t>A Hapvida e o Grupo NotreDame Intermédica realizarão um webcast para discutir as sinergias da fusão aprovada pelo CADE.</t>
+  </si>
+  <si>
+    <t>Hapvida NotreDame Intermédica tem 200 vagas para curso gratuito em TI - Estado de Minas</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMimAFodHRwczovL3d3dy5lbS5jb20uYnIvYXBwL25vdGljaWEvZW1wcmVnby8yMDIyLzExLzAzL2ludGVybmFfZW1wcmVnbywxNDE2NjE0L2hhcHZpZGEtbm90cmVkYW1lLWludGVybWVkaWNhLXRlbS0yMDAtdmFnYXMtcGFyYS1jdXJzby1ncmF0dWl0by1lbS10aS5zaHRtbNIBVWh0dHBzOi8vd3d3LmVtLmNvbS5ici9hcHAvbm90aWNpYS9lbXByZWdvLzIwMjIvMTEvMDMvaW50ZXJuYV9lbXByZWdvLDE0MTY2MTQvYW1wLmh0bWw?oc=5</t>
+  </si>
+  <si>
+    <t>Estado de minas</t>
+  </si>
+  <si>
+    <t>Para participar do Programa One, os interessados devem ter idade mínima de 18 anos (foto: Gerd Altmann/Pixabay )
+LEIA MAIS 12:45 - 01/11/2022 Concurso TRT-8: número de inscritos é superior a 30 mil
+10:48 - 01/11/2022 Concurso para PMCE: edital de abertura é publicado com 300 vagas
+11:03 - 31/10/2022 Edital do concurso do Ministério Público de MG é retificado O Hapvida NotreDame Intermédica começou a formar profissionais oriundos de minorias sociais para integrá-los ao mercado de tecnologia da informação e aos próprios quadros do grupo. O projeto faz parte do Programa One, desenvolvido pela Oracle, e consiste em um curso on-line de qualificação em TI, de seis meses, com perspectiva de contratação pela companhia. As inscrições estão abertas desde 01/11.O público-alvo envolve pessoas com deficiência física e psicológica, negras, LGBTQIA+ e com mais de 50 anos. A primeira turma conta com 30 participantes de Fortaleza e uma nova, com 200 vagas, está sendo aberta para alunos de todo o país.
+Leia também:
+Para participar do Programa One, os interessados devem ter idade mínima de 18 anos; estar cursando ou ter concluído o ensino médio em escola pública (ou particular com bolsa); não ter e nem cursar nível superior; não estar trabalhando com
+A ação reforça o planejamento estratégico ESG do grupo — que acaba de aderir à Rede Empresarial de Inclusão Social, reunindo corporações comprometidas com a ampliação do mercado de trabalho para deficientes no Brasil. O One (Oracle Next Education) conta com aulas semanais, com pelo menos três horas de duração, totalmente on-line e gratuitas. Além disso, há tira-dúvidas ao vivo.Leia também: Senac tem mais de 11 mil vagas para cursos técnicos gratuitos e a distância. Para participar do Programa One, os interessados devem ter idade mínima de 18 anos; estar cursando ou ter concluído o ensino médio em escola pública (ou particular com bolsa); não ter e nem cursar nível superior; não estar trabalhando com tecnologia da informação ou desenvolvimento de sistemas; ter acesso à internet e a um computador para assistir às aulas do curso, e disponibilidade de tempo para estudar.
+Chance de contratação
+Após o curso, os alunos terão o seu desempenho avaliado para possível contratação de acordo com as vagas disponíveis nas unidades do grupo Hapvida NotreDame Intermédica.
+"O Programa One reflete nossa política de diversidade e queremos ampliá-la ainda mais numa área carente de talentos no Brasil, como é a de TI. Isso é bom para todos porque ganharemos profissionais com visões de mundo diversas e ajudaremos a formar uma sociedade ainda mais justa ao promovermos ainda mais a “Somos uma empresa multicultural e diversa, tal como a sociedade, e queremos descobrir e receber os grandes talentos entre grupos sociais que necessitam de ações públicas e privadas de afirmação. Precisamos abrir as portas do mercado a esses profissionais e é isso que queremos fazer", explica o diretor de gente, gestão e diversidade do Hapvida NotreDame Intermédica, Ricardo Mota."O Programa One reflete nossa política de diversidade e queremos ampliá-la ainda mais numa área carente de talentos no Brasil, como é a de TI. Isso é bom para todos porque ganharemos profissionais com visões de mundo diversas e ajudaremos a formar uma sociedade ainda mais justa ao promovermos ainda mais a inclusão social nos nossos quadros", destaca Ricardo Mota.
+"O Hapvida NotreDame Intermédica tem a diversidade e a inclusão social como partes vitais em seu planejamento estratégico. Isso transforma o ambiente empresarial, que precisa estar em conformidade com a sociedade que o cerca e nos ajuda a evoluir porque, abraçando a diversidade, nós nos tornamos ainda mais inovadores por estarmos abertos a diferentes formas de pensar e olhar para o outro e o ambiente em que vivemos”, define o vice-presidente de ASG da companhia, João Alceu.</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) S (Social).
+c) +0.9. A notícia tem um sentimento muito positivo, destacando ações de inclusão social e diversidade.
+d) Hapvida NotreDame Intermédica.
+e) Sim, o tema principal é a empresa "notredame intermedica".
+f) A Hapvida NotreDame Intermédica oferece 200 vagas em um curso gratuito de TI focado em minorias sociais, com perspectiva de contratação, reforçando seu compromisso com a inclusão social.</t>
+  </si>
+  <si>
+    <t>ba23460eb3713ecd6a35310df3276de153baecd7ef8be3f57fc5f01216cdfad3</t>
+  </si>
+  <si>
+    <t>['ESG', 'S', 0.9, 'Hapvida NotreDame Intermédica', 'Sim', 'A Hapvida NotreDame Intermédica oferece 200 vagas em um curso gratuito de TI focado em minorias sociais, com perspectiva de contratação, reforçando seu compromisso com a inclusão social.']</t>
+  </si>
+  <si>
+    <t>Hapvida NotreDame Intermédica</t>
+  </si>
+  <si>
+    <t>A Hapvida NotreDame Intermédica oferece 200 vagas em um curso gratuito de TI focado em minorias sociais, com perspectiva de contratação, reforçando seu compromisso com a inclusão social.</t>
+  </si>
+  <si>
+    <t>Diretora da Hapvida fala sobre os aprendizados em digitalização - Consumidor Moderno</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiOWh0dHBzOi8vY29uc3VtaWRvcm1vZGVybm8uY29tLmJyL2hhcHZpZGEtam9ybmFkYS1kaWdpdGFsL9IBAA?oc=5</t>
+  </si>
+  <si>
+    <t>A digitalização e a expansão dos canais de atendimento faziam parte do planejamento estratégico das empresas de diversos portes e setores no pré-pandemia, e foram priorizados no cenário de distanciamento social vivenciado no período mais crítico da Covid-19.
+De lá para cá, essas interações entre marcas e clientes ganharam novos contornos e hoje toda empresa foco suas atenções para o atendimento mais humano, resolutivo e ágil – seja no ambiente digital ou físico.
+Especificamente no setor de saúde, a Teleconsulta, inicialmente, evitou o deslocamento dos pacientes até as unidades de saúde, minimizando os riscos de contaminação e, hoje, garante acesso ágil à saúde especializada para milhares de pessoas.
+No grupo Hapvida NotreDame Intermédica, por exemplo, seus beneficiários em regiões distantes dos grandes centros, encontram na teleconsulta a orientação médica ideal e de qualidade, além do acolhimento na relação médico-paciente tão importante nos dias atuais.
+Essas características são fundamentais no relacionamento com clientes agora, mas, principalmente no setor da saúde, o contato humano ainda é preponderante para o sucesso e resolutividade do atendimento ao cliente.
+“O fator humano continua sendo valorizado, independente do ponto de contato, por isso, o processo de automatização dos canais de atendimento deve resolver as principais “dores” dos clientes como comodidade, agilidade e, principalmente, resolutividade de forma simples e segura”, avalia Adria Candido, diretora corporativa de saúde digital e clínicas médicas da Hapvida.
+Conheça o Mundo do CX
+“O principal desafio é acelerar a integração de todos os canais e a utilização dos dados para prover as melhores experiências”
+Digitalização: uma jornada de aprendizados
+Segundo Adria, o grande aprendizado da jornada de digitalização é que os novos canais de atendimento vêm somar a estratégia de multicanalidade e não substituir pontos de contato tradicionais. “A adoção e perpetuação de alguns canais dependem de mudanças culturais e socioeconômicas, por isso, requer tempo, comunicação assertiva e fases de experimentação dos clientes”, pontua a diretora da Hapvida.
+Nesse caminho, o grupo Hapvida NotreDame Intermédica, realizou diversas ações para que seus beneficiários conhecessem a telemedicina e seus benefícios. Ao longo desse processo, até hoje, já foram realizados mais de 4 milhões de atendimentos digitais com desfechos clínicos favoráveis, sem a necessidade de deslocamento.
+“Agora, o principal desafio é acelerar a integração de todos os canais e a utilização dos dados para prover as melhores experiências em todos eles, seja no digital ou presencial, isto é, garantindo a omnicanalidade e, genuinamente, um modelo de operação phygital”, explica Adria Candido.
+Um ponto importante nessa análise sobre a digitalização e humanização do atendimento no setor de saúde é a acessibilidade. Segundo Adria, a utilização de novas tecnologias está mais acessível, o que possibilita o teste e adoção de diversas ferramentas, porém, a verdadeira solução está em entender as necessidades e desejos dos clientes, seus níveis de satisfação e lealdade às marcas.
+“Com a melhora do cenário de conectividade, emprego e renda da população, o uso da telemedicina na saúde suplementar tende a ganhar mais impulso”, avalia Adria.
+Para a diretora, toda essa evolução e vivência do setor de saúde nos últimos anos com a aceleração da digitalização, levou as empresas a entenderem melhor o comportamento de seus clientes.
+“Conhecer os clientes, perfis e comportamento, suas necessidades, desejos e expectativas é o primeiro passo para prover um atendimento digital de qualidade, visto que as tecnologias são meio para prover experiências memoráveis”, conclui a executiva.
++ Notícias
+A difícil arte (e a menosprezada ciência) de respeitar o cliente
+Atendimento aos millennials demanda respeito e adequação aos ideais sociais, políticos e ambientais</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) A dimensão dominante é S.
+c) O sentimento da notícia é positivo, avaliado em +0.8.
+d) Hapvida NotreDame Intermédica.
+e) Sim, o texto tem como tema principal a empresa "notredame intermedica".
+f) A Hapvida NotreDame Intermédica foca na digitalização e humanização do atendimento, promovendo acessibilidade e qualidade na saúde através da teleconsulta.</t>
+  </si>
+  <si>
+    <t>40c4a93ec8cefeb3fcdefbf130ef9a1a4e99551967edfd6c486360b1c7e301cb</t>
+  </si>
+  <si>
+    <t>['ESG', 'S', 0.8, 'Hapvida NotreDame Intermédica', 'Sim', 'A Hapvida NotreDame Intermédica foca na digitalização e humanização do atendimento, promovendo acessibilidade e qualidade na saúde através da teleconsulta.']</t>
+  </si>
+  <si>
+    <t>A Hapvida NotreDame Intermédica foca na digitalização e humanização do atendimento, promovendo acessibilidade e qualidade na saúde através da teleconsulta.</t>
+  </si>
+  <si>
+    <t>EDP e Hapvida NotreDame Intermédica firmam parceria para geração de energia solar - Correio Braziliense</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMitAFodHRwczovL3d3dy5jb3JyZWlvYnJhemlsaWVuc2UuY29tLmJyL3BhcmNlaXJvcy9oYXB2aWRhLW5vdHJlZGFtZS1pbnRlcm1lZGljYS8yMDIyLzExLzUwNTQ1ODgtZWRwLWUtaGFwdmlkYS1ub3RyZWRhbWUtaW50ZXJtZWRpY2EtZmlybWFtLXBhcmNlcmlhLXBhcmEtZ2VyYWNhby1kZS1lbmVyZ2lhLXNvbGFyLmh0bWzSAbgBaHR0cHM6Ly93d3cuY29ycmVpb2JyYXppbGllbnNlLmNvbS5ici9wYXJjZWlyb3MvaGFwdmlkYS1ub3RyZWRhbWUtaW50ZXJtZWRpY2EvMjAyMi8xMS9hbXAvNTA1NDU4OC1lZHAtZS1oYXB2aWRhLW5vdHJlZGFtZS1pbnRlcm1lZGljYS1maXJtYW0tcGFyY2VyaWEtcGFyYS1nZXJhY2FvLWRlLWVuZXJnaWEtc29sYXIuaHRtbA?oc=5</t>
+  </si>
+  <si>
+    <t>Correio braziliense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentado por
+(crédito: Divulgação Hapvida NotreDame Intermédica.)
+Em uma iniciativa pioneira no setor de saúde do Brasil, a Hapvida NotreDame Intermédica, maior grupo de saúde e odontologia do Brasil; e o grupo EDP, um dos líderes globais em energias renováveis, firmaram contrato com duração de 15 anos para a autoprodução de 30,50 MWac de energia solar, o que deve suprir cerca de 85% da demanda de energia das unidades da NotreDame Intermédica nos próximos anos.
+A usina fotovoltaica, localizada no estado de São Paulo, é uma parceria com co-investimento 50%/50% entre a EDP Brasil e a EDP Renováveis, as duas empresas do grupo que operam no país. A transação aguarda aprovação do Conselho de Administração para Defesa Econômica (CADE).
+"A iniciativa é extremamente significativa e simbólica, pois coloca a Hapvida NotreDame Intermédica na vanguarda do setor de saúde, quando o assunto é a autoprodução de energia solar." João Alceu Amoroso Lima, vice-presidente de Ambiental, Social e Governança (ASG) do Grupo Hapvida NotreDame Intermédica.
+A empresa, nos dois últimos anos, tornou-se "carbono neutro" com a compensação de 100% das suas emissões de gases de efeito estufa e obteve a nota B- no CDP Climate Change, a melhor do setor de saúde brasileiro.
+Além do contrato de autoprodução, a EDP e a Hapvida NotreDame Intermédica firmaram parceria para a migração das unidades do grupo de saúde para o mercado livre de energia e para o fornecimento de energia para essas unidades até a entrada em operação da usina solar, a partir de 2024.
+(foto: Divulgação Hapvida NotreDame Intermédica.)
+“No total, 64 unidades, incluídas na estrutura de autoprodução, fizeram parte da migração do mercado regulado da operadora”, reforça Amoroso Lima. A EDP está construindo também cinco usinas solares de Geração Distribuída que irão abastecer 55% das unidades da Hapvida NotreDame Intermédica que operam em baixa tensão.
+“O sucesso da EDP no desenvolvimento de novos modelos de negócio e de projetos de longo prazo, com oferta de soluções integradas direcionadas aos clientes, reforça o perfil inovador e sustentável e a estratégia de crescimento pautada na aceleração da transição energética e na descarbonização da economia”, reforça Carlos Andrade, vice-presidente de Clientes da EDP no Brasil.
+Tanto Hapvida quanto NotreDame Intermédica já possuíam parcerias para geração de energias renováveis, anteriormente. Trata-se de uma cultura das organizações. O Hapvida, pelo menos desde 2020, trabalha com fontes de energias renováveis, tanto com geração distribuída como no mercado livre. E a NotreDame Intermédica firmou, em abril de 2021, o contrato com a EDP.
+Sobre o Grupo EDP no Brasil
+Presente em 29 mercados, o Grupo EDP está no Brasil há mais de 25 anos por meio das empresas EDP Brasil e EDP Renováveis, com R$ 41 bilhões em ativos no país, caracterizando essa como a segunda maior operação da companhia no mundo. Até 2025, o grupo deve investir cerca de R$ 18,2 bilhões no país, sendo R$ 5,7 bilhões em energia solar. A companhia conta com mais de 10 mil colaboradores diretos e terceirizados no Brasil e atua nos segmentos de geração, transmissão, distribuição e comercialização de energia, além do desenvolvimento, construção e manutenção de ativos eólicos e solares.
+A empresa oferece também soluções de energia voltadas ao mercado B2B, como geração solar distribuída, mobilidade elétrica e venda de energia no mercado livre. Na Distribuição, a EDP atende a cerca de 3 milhões de clientes em São Paulo e no Espírito Santo. Em 2022, foi eleita pelo terceiro ano consecutivo a empresa mais inovadora do setor elétrico pelo ranking Valor Inovação, do jornal Valor Econômico, e é referência em ESG, ocupando, em 2021, o primeiro lugar do Índice de Sustentabilidade Empresarial (ISE) da B3, no qual figura há 16 anos.
+Sobre o Grupo Hapvida NotreDame Intermédica
+Resultante da fusão entre Hapvida e a NotreDame Intermédica, em 2022, formou-se o maior grupo de saúde e odontologia do Brasil. Os números superlativos do Grupo Hapvida NDI mostram o sucesso da operação que reúne cerca de 15 milhões de clientes, mais de 65 mil colaboradores, 7 mil leitos de atendimento hospitalar e 18% de participação de mercado em planos de saúde. Presente nas cinco regiões do País, a rede própria de atendimento conta com 85 hospitais, 77 Prontos Atendimentos, 318 clínicas médicas e 269 centros de diagnóstico por imagem e coleta laboratorial. Dessa fusão, apoiada em inovação, resulta uma empresa com os melhores recursos humanos e tecnológicos para os seus clientes.
+</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.  
+b) A dimensão dominante é E (Ambiental).  
+c) O sentimento da notícia é positivo, avaliado em +0.8.  
+d) As principais empresas envolvidas são Hapvida NotreDame Intermédica e EDP.  
+e) Sim, o texto tem como tema principal a empresa "notredame intermedica".  
+f) Hapvida NotreDame Intermédica e EDP firmam parceria para a geração de energia solar, visando suprir 85% da demanda energética das unidades da NotreDame Intermédica, destacando o compromisso ambiental e a inovação no setor de saúde.</t>
+  </si>
+  <si>
+    <t>e807fce066b1491ff48179f3a6fa4b92114db6e4a181b5d90d79431a0aa32d1f</t>
+  </si>
+  <si>
+    <t>['ESG', 'E', 0.8, 'As principais empresas envolvidas são Hapvida NotreDame Intermédica e EDP  ', 'Sim', 'Hapvida NotreDame Intermédica e EDP firmam parceria para a geração de energia solar, visando suprir 85% da demanda energética das unidades da NotreDame Intermédica, destacando o compromisso ambiental e a inovação no setor de saúde.']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As principais empresas envolvidas são Hapvida NotreDame Intermédica e EDP  </t>
+  </si>
+  <si>
+    <t>Hapvida NotreDame Intermédica e EDP firmam parceria para a geração de energia solar, visando suprir 85% da demanda energética das unidades da NotreDame Intermédica, destacando o compromisso ambiental e a inovação no setor de saúde.</t>
+  </si>
+  <si>
+    <t>Reembolso de planos amplia debate sobre direito dos pacientes e de operadoras - JOTA</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMihgFodHRwczovL3d3dy5qb3RhLmluZm8vdHJpYnV0b3MtZS1lbXByZXNhcy9zYXVkZS9yZWVtYm9sc28tZGUtcGxhbm9zLWFtcGxpYS1kZWJhdGUtc29icmUtZGlyZWl0by1kb3MtcGFjaWVudGVzLWUtZGUtb3BlcmFkb3Jhcy0wMjEyMjAyMtIBigFodHRwczovL3d3dy5qb3RhLmluZm8vdHJpYnV0b3MtZS1lbXByZXNhcy9zYXVkZS9yZWVtYm9sc28tZGUtcGxhbm9zLWFtcGxpYS1kZWJhdGUtc29icmUtZGlyZWl0by1kb3MtcGFjaWVudGVzLWUtZGUtb3BlcmFkb3Jhcy0wMjEyMjAyMi9hbXA?oc=5</t>
+  </si>
+  <si>
+    <t>Jota</t>
+  </si>
+  <si>
+    <t>Crédito Pixabay
+JOTA PRO Saúde Este conteúdo integra a cobertura do JOTA PRO Saúde e foi distribuído antes com exclusividade para assinantes PRO. Conheça!
+A decisão da 3ª Turma do Superior Tribunal de Justiça (STJ) no dia 22/11 de que planos de saúde só precisam reembolsar exames e consultas se houver pagamento direto por parte dos pacientes provocou debate em torno dos direitos dos consumidores e das operadoras. Os ministros reformaram o entendimento do Tribunal de Justiça de São Paulo (TJSP) de que a prática era possível.
+Um dos argumentos do relator, ministro Marco Aurélio Bellizze, é de que não estava estabelecido, de fato, o direito ao reembolso, mas uma mera expectativa dele. “O direito ao reembolso depende por pressuposto lógico que o beneficiário tenha, efetivamente, desembolsado previamente os valores com a assistência à saúde, sendo imprescindível, ainda, o preenchimento dos demais requisitos previstos na Lei de Planos de Saúde. Antes disso, mera expectativa de direito”, afirmou o relator em seu voto.
+O caso — REsp 1.959.929/SP (2021/0021933-3) — se refere a uma ação da Notre Dame Intermédica Saúde S/A contra a Clínica Corpo Saudável e o laboratório Bem Estar Serviços e Diagnósticos, que realizavam consultas e exames sem pagamento prévio. Quando a operadora liberava o valor, o reembolso era repassado para as empresas.
+“Se o usuário não despendeu nenhum valor a título de despesas médicas, mostra-se incabível a transferência do direito ao reembolso, visto que, na realidade, esse direito sequer existia, o negócio jurídico firmado entre a clínica, o laboratório e os segurados, cessão de direito ao reembolso sem prévio desembolso, operou-se sem objeto, o que o torna nulo de pleno direito”, sustentou Bellizze. Os demais magistrados seguiram o entendimento dele, levando a uma decisão unânime.
+Debate
+Nesse sentido, a advogada Ingrid Belian vê a decisão como acertada: “A decisão do STJ está de acordo com a Lei dos Planos de Saúde, porque restabelece as regras de quem pode fazer e solicitar o reembolso e as normas diferenciadas para clínicas credenciadas ou não”, comenta a especialista em Direito Médico e em Bioética.
+Na avaliação da União Nacional das Instituições de Autogestão em Saúde (Unidas), que representa mais de 100 operadoras, a prática de pedir reembolso antes que o pagamento tenha sido de fato feito representa uma espécie de fraude:
+“É uma fraude processual, porque o reembolso é caracterizado a partir do pagamento: você reembolsa alguém que pagou alguma coisa. Então, você não pode ter um reembolso de um serviço pelo qual não pagou. A relação contratual é do beneficiário com a operadora. As clínicas particulares que não são credenciadas não têm essa relação”, disse ao JOTA o presidente da Unidas, Anderson Mendes.
+Apesar da pressuposição de que o reembolso só existiria após o prévio desembolso, tal posicionamento poderia ir na contramão do direito dos consumidores:
+“Existe essa pressuposição lógica que está de acordo com a sistemática, só que essa decisão pode vir a impactar a livre escolha do paciente. Alguns deles não têm como desembolsar previamente o valor de um procedimento cirúrgico, por exemplo”, diz a advogada Thaís Maia, sócia do Maia &amp; Munhoz Consultoria e Advocacia em Biodireito e Saúde.</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) G (Governança).
+c) -0.2. A notícia mostra uma decisão judicial que pode limitar o acesso dos consumidores a reembolsos por serviços de saúde, o que pode ser visto como negativo sob a ótica de direitos do consumidor, mas é justificado pela necessidade de evitar fraudes.
+d) Notre Dame Intermédica Saúde S/A.
+e) Sim, o texto tem como tema principal a empresa "Notre Dame Intermédica".
+f) A decisão do STJ sobre reembolsos de planos de saúde, envolvendo a Notre Dame Intermédica, levanta questões sobre direitos dos consumidores e práticas de operadoras para evitar fraudes.</t>
+  </si>
+  <si>
+    <t>5da173428e2a9ef485cd67ba5184592e07a3908e91ee1e16f23723a6aaa21a30</t>
+  </si>
+  <si>
+    <t>['ESG', 'G', -0.2, 'Notre Dame Intermédica Saúde S/A', 'Sim', 'A decisão do STJ sobre reembolsos de planos de saúde, envolvendo a Notre Dame Intermédica, levanta questões sobre direitos dos consumidores e práticas de operadoras para evitar fraudes.']</t>
+  </si>
+  <si>
+    <t>Notre Dame Intermédica Saúde S/A</t>
+  </si>
+  <si>
+    <t>A decisão do STJ sobre reembolsos de planos de saúde, envolvendo a Notre Dame Intermédica, levanta questões sobre direitos dos consumidores e práticas de operadoras para evitar fraudes.</t>
+  </si>
+  <si>
+    <t>Consciência negra: campanha da Hapvida NotreDame Intermédica reforça a importância do combate à discriminação - saudebusiness.com</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMie2h0dHBzOi8vd3d3LnNhdWRlYnVzaW5lc3MuY29tL29wZXJhZG9yYXMvY29uc2NpZW5jaWEtbmVncmEtY2FtcGFuaGEtZGEtaGFwdmlkYS1ub3RyZWRhbWUtaW50ZXJtZWRpY2EtcmVmb3JjYS1pbXBvcnRhbmNpYS1kb9IBAA?oc=5</t>
+  </si>
+  <si>
+    <t>Saudebusiness.com</t>
+  </si>
+  <si>
+    <t>Hoje, no Brasil, 56% da população é negra, conforme o Instituto Brasileiro de Geografia e Estatística (IBGE). Entretanto, dados do Anuário Brasileiro de Segurança Pública mostram uma triste realidade, que aponta crescimento de 67% nos registros de crimes de racismo em 2022, frente ao ano anterior.
+Para reforçar a importância do combate diário a todo tipo de discriminação, a Hapvida NotreDame Intermédica lança a campanha “A transformação só acontece com a sua atitude”, alusiva ao Dia da Consciência, celebrado em 20 de novembro. A iniciativa inclui cartilha informativa, reforço de treinamentos sobre diversidade, equidade e inclusão; vídeo elaborado pelos funcionários da instituição sobre situações cotidianas em que o racismo se expressa, além do incentivo à participação no grupo de afinidade étnico-racial da companhia.
+Relacionado: Hapvida NotreDame Intermédica amplia rede de atendimento com três novos hospitais
+Além do desenvolvimento da campanha, diversos dados reforçam a trajetória de evolução na cultura de inclusão da empresa: dos 66 mil colaboradores, 61% são pessoas pretas ou pardas. E mais: de todas as lideranças da instituição, 48% são pessoas negras. “Números e metas são importantes para sabermos onde estamos e para onde vamos. Mas, acima de tudo, somos uma empresa de pessoas feita para pessoas e o nosso jeito de ser é acolher todas elas com o devido e merecido respeito”, afirma o diretor de Comunicação Corporativa e Diversidade da Hapvida NotreDame Intermédica, Ricardo Mota. Para o executivo, os valores da companhia vão ao encontro do propósito de avançar como sociedade: “Trabalhamos para salvar vidas. Isso não é uma escolha: e sim a nossa nobre missão”, reforça.
+Lideranças
+Dentre as 1,7 mil lideranças negras da Hapvida NotreDame Intermédica, está a Head de Inovação Aberta, Ana Carolina Cândido, de 34 anos, que compartilha a sua história inspiradora de 13 anos na gestão de saúde. “Sempre tive uma inquietação pessoal por saber que muitos avanços da ciência e da tecnologia não chegavam até as pessoas. Por essa razão, comecei a enxergar na inovação a possibilidade de conectar a população às condutas assistenciais personalizadas, efetivas e remotas, quando necessárias”, informa.
+Divulgação Ana Carolina, Head de Inovação Aberta: "tenha a intenção de gerar transformação com seus atos".
+Gestora do portfólio de startups desde 2021, Ana é responsável pelas ações de Inovação Aberta e Posicionamento dentro do time de Inovação e atribui a trajetória de sucesso à busca pelo autoconhecimento e a ser intencional em cada ação. “Saber quem você é, de onde você veio, conhecer a sua história, ter clareza da sua jornada e da jornada de seus ancestrais te dará mais base e força para buscar seus objetivos e passar pelos desafios do dia a dia, que são muitos. Não faça nada só por fazer, tenha a intenção de gerar mudança e transformação com os seus atos; mesmo os pequenos gestos geram movimento em grandes estruturas”, reflete.
+Outra trajetória de inspiração é a da consultora de RH Eliana Santos das Neves, de 38 anos, que iniciou a jornada na empresa há nove anos como assistente e foi reconhecida por participar ativamente de todos os processos da área e evoluir constantemente.
+Para a colaboradora, a cultura de inclusão e diversidade é um processo de reconhecimento, conscientização, aceitação, valorização das diferenças entre as pessoas e equidade de oportunidades. “Sinto muito orgulho em ver a empresa trilhando os caminhos da diversidade e da inclusão, trazendo a importância de falar sobre a pauta e, principalmente, demonstrar por meio de seus posicionamentos e ações o incentivo à participação e contratação de grupos diversos”, ressalta.
+Para o diretor regional Valfredo Amaro, de 56 anos, a sua trajetória de mais de duas décadas é um motivo de orgulho. “Fui cliente e vendedor da Hapvida por alguns anos antes de ser colaborador, o que me ajudou a entender a qualidade do serviço, do atendimento e do acolhimento prestados”, compartilha. Após conquistar vaga efetiva, Amaro seguiu crescendo na empresa e hoje é gestor sênior, responsável por vendas comerciais. Para o executivo, a essência da companhia é a pluralidade e a natureza acolhedora, com foco no propósito de levar saúde de qualidade por preços justos à população. “A cor de pele, a idade e a orientação sexual não impedem de se chegar a qualquer lugar nesta companhia, pois o objetivo da empresa é o trabalho com foco no cliente", afirma.
+Por fim, Mota destaca a importância da diversidade e da inclusão para a companhia e para o País: “Estamos comprometidos na construção desta nova sociedade e seguimos juntos nesta jornada de construção e conquistas”, sintetiza.</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) S (Social).
+c) +1.0.
+d) Hapvida NotreDame Intermédica.
+e) Sim.
+f) A Hapvida NotreDame Intermédica lança campanha para combater a discriminação e reforçar a importância da diversidade e inclusão, destacando ações internas e a representatividade negra na empresa.</t>
+  </si>
+  <si>
+    <t>9ebe170c1853b15bb68e4c1f85b8935e398c72cd995b4222e9fb39706ef4d86c</t>
+  </si>
+  <si>
+    <t>['ESG', 'S', 1.0, 'Hapvida NotreDame Intermédica', 'Sim', 'A Hapvida NotreDame Intermédica lança campanha para combater a discriminação e reforçar a importância da diversidade e inclusão, destacando ações internas e a representatividade negra na empresa.']</t>
+  </si>
+  <si>
+    <t>A Hapvida NotreDame Intermédica lança campanha para combater a discriminação e reforçar a importância da diversidade e inclusão, destacando ações internas e a representatividade negra na empresa.</t>
+  </si>
+  <si>
+    <t>Notredame diz ser alvo do excesso de judicialização - Consumidor Moderno</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiQmh0dHBzOi8vY29uc3VtaWRvcm1vZGVybm8uY29tLmJyL25vdHJlZGFtZS1leGNlc3NvLWp1ZGljaWFsaXphY2FvL9IBAA?oc=5</t>
+  </si>
+  <si>
+    <t>A empresa Hapvida Notredame está sendo investigada pelo Ministério Público de São Paulo (MPSP) por suposto descumprimento de decisões judiciais que determinavam tratamento e o fornecimento de medicamentos a clientes. O inquérito, das esferas cível e criminal, foi instaurado pela Promotoria de Justiça do Consumidor do MPSP, e vai apurar a recusa de atendimento a pacientes.
+A rejeição ao atendimento médico ou hospitalar agride a dignidade do paciente e de seus familiares, e pode ser considerada uma violação ao dever de informação e à boa-fé objetiva, de acordo com a Lei nº 8.078/1990. É importante destacar que a Lei nº 9.596/1998 também prevê a obrigação de cobertura em casos de atendimento de urgência ou emergência.
+Independentemente de questões burocráticas, a recusa ao atendimento coloca em risco a vida do paciente, o que vai contra um princípio fundamental. Foi o que aconteceu com a dona de casa Matilde Ramos, de 60 anos, que morreu no dia 10 de outubro do ano passado após ter uma cirurgia de urgência negada na rede hospitalar do convênio com a Notredame Intermédica, mesmo após conseguir uma liminar favorável.
+Entenda o caso da denúncia contra a Notredame
+Matilde Ramos procurou atendimento médico com queixa de dores abdominais e pele e olhos amarelados (icterícia). Na ocasião, exames apontaram a necessidade de retirada da vesícula. Na operadora, mesmo com o pedido médico em mãos, Matilde teve a cirurgia negada. A argumentação foi que o contrato estava ainda em período de carência.
+A paciente então ingressou com pedido de liminar na Justiça e recebeu decisão favorável no dia 12 de setembro. No despacho, o juiz obrigou a operadora a realizar a operação em até três dias e fixou multa de R$ 500 por dia de descumprimento.
+O inquérito do MPSP
+O promotor Cesar Ricardo Martins afirmou que as informações trazidas aos autos entram em conflito com a Política Nacional das Relações de Consumo. Tal Política visa atender as necessidades dos consumidores, “respeitar sua dignidade, saúde e segurança, proteger seus interesses econômicos, melhorar sua qualidade de vida, e promover transparência e harmonia nas relações de consumo”, cita ele na portaria de instauração do inquérito, de 12 de janeiro de 2024.
+O MPSP abriu também duas investigações criminais para apurar a possibilidade de a empresa Hapvida ter cometido o crime de desobediência ao ignorar decisões judiciais. Uma das investigações foi iniciada pela promotoria de Jundiaí em agosto do ano passado e foi prorrogada em novembro. A outra investigação, aberta em Osasco, foi arquivada em setembro de 2023.
+A fusão das operadoras Hapvida e Notredame ocorreu em 2022. Desde então, 63% das decisões judiciais foram descumpridas. O Ministério Público identificou um comportamento resistente que é mais comum em casos de câncer, cirurgias e tratamentos de autismo em crianças.
+A Hapvida NotreDame Intermédica é, hoje, a maior operadora de saúde do Brasil, com mais de 16 milhões de beneficiários de saúde e odontologia.
+As ações da Hapvida Notredame na Bolsa de Valores
+Na B3, no dia 18 de janeiro, as ações da Hapvida – HAPV3 – registraram queda de -6,98%. Essa foi a menor cotação desde novembro de 2023. Diante dos fatos, sites para investidores, como o Nordinvestimentos, por exemplo, aconselham seus leitores a ficarem fora desses papéis. “A companhia não conseguiu manter um crescimento consistente de Ebitda, com uma piora mais recente, além de apresentar queda de lucros desde 2018, e atualmente reportou prejuízo em seus resultados”.
+A Associação Brasileira de Planos de Saúde (Abramge) destaca a importância da segurança jurídica nos contratos entre beneficiários e operadoras de saúde. Para ela, as “demandas judiciais, a alta sinistralidade e a má utilização dos planos têm sido desafios para o setor”.
+Ademais, como a alta judicialização afeta o atendimento à sociedade, a Associação destaca que o acesso ao sistema judicial é um direito garantido a todos, mas que as demandas individuais devem estar respaldadas por bases legais, regulatórias e contratuais.
+Democratização do acesso à saúde
+A Notredame esclarece que segue firme em seu propósito de democratizar o acesso à saúde de qualidade para quase 15 milhões de pessoas. Suas premissas são o cuidado, o acolhimento, a acessibilidade, a segurança e o cumprimento das normas aplicáveis. Para isso, a empresa se mantém focada em prestar um atendimento cada vez melhor em seu contínuo processo de aperfeiçoamento.
+Os números da Companhia mostram a envergadura e a capilaridade: em 2023, por exemplo, ela realizou mais de 40 milhões de consultas e cerca de 83 milhões de exames. Apenas em atendimento oncológico, ela prestou assistência para mais de 32 mil beneficiários. O total de cirurgias, apenas na rede própria, ultrapassa 277 mil.
+Judicialização e suas complexidades
+A companhia ressalta ainda os estudos recentes realizados por associações e institutos do setor de saúde suplementar, como Instituto de Estudos de Saúde Suplementar (IESS) e a Abramge, que reconhecem os impactos da crescente judicialização e suas complexidades.
+O expediente vem sendo utilizado mesmo antes de uma conciliação através dos canais oferecidos pelas operadoras e pela Agência Nacional de Saúde Suplementar (ANS).
+“Em muitas situações, os pedidos envolvem fraudes e solicitações de coberturas não abrangidas por lei e/ou o respectivo contrato, inclusive sem o devido cumprimento do período de carência. Conforme apontado por estudos setoriais, esse tipo de judicialização gera um prejuízo sistêmico, refletindo, por exemplo, em reajustes nos planos de saúde de todos os beneficiários, fruto de um descolamento entre a inflação médica e a inflação ampla”, diz a Hapvida Notredame.
+Por fim, a Notredame informa que tomou conhecimento da investigação junto ao Ministério Público por meio da Promotoria de Defesa do Consumidor. Com acesso aos autos, ela contribuirá e prestará ativamente os esclarecimentos necessários de forma tempestiva mantendo sua prática de respeito ao Poder Judiciário.
+Números
+No terceiro trimestre do ano passado, a Hapvida reportou um lucro líquido de R$ 261,1 milhões, encerrando o período com 15.848 beneficiários. Portanto, houve uma diminuição anual de 0,4%, e 68 mil planos de saúde ou odontológicos a menos do que em 2022. O valor médio por beneficiário foi de R$ 251,80, um aumento de 11,8%.
+O Índice de Desempenho da Saúde Suplementar de 2023, com base em 2022, aponta que as operadoras da Hapvida NotreDame Intermédica conquistaram a melhor faixa de pontuação. Esse índice é resultado da avaliação do Programa de Qualificação de Operadoras, da ANS. Assim, no ano passado, a Hapvida Assistência Médica S.A. e Notre Dame Intermédica Saúde S.A., receberam 0,802 e 1, respectivamente (escala de 0 a 1, sendo zero a menor nota e 1 a maior).</t>
+  </si>
+  <si>
+    <t>a) Sim, a notícia é do tema ESG.
+b) A dimensão dominante é S (Social).
+c) -0.8. A atitude da empresa sob a ótica ESG é vista de forma negativa, principalmente devido ao descumprimento de decisões judiciais e à negação de tratamentos médicos necessários.
+d) Hapvida Notredame.
+e) Sim, o texto tem como tema principal a empresa "Notredame Intermédica".
+f) A Hapvida Notredame está sendo investigada pelo MPSP por suposto descumprimento de decisões judiciais relacionadas ao tratamento e fornecimento de medicamentos a clientes, afetando negativamente sua reputação e ações na bolsa.</t>
+  </si>
+  <si>
+    <t>09990153c6f3b4b944e9b0657aac71fdd000ade0993a8cb9868e79bdcd76d2de</t>
+  </si>
+  <si>
+    <t>['ESG', 'S', -0.8, 'Hapvida Notredame', 'Sim', 'A Hapvida Notredame está sendo investigada pelo MPSP por suposto descumprimento de decisões judiciais relacionadas ao tratamento e fornecimento de medicamentos a clientes, afetando negativamente sua reputação e ações na bolsa.']</t>
+  </si>
+  <si>
+    <t>Hapvida Notredame</t>
+  </si>
+  <si>
+    <t>A Hapvida Notredame está sendo investigada pelo MPSP por suposto descumprimento de decisões judiciais relacionadas ao tratamento e fornecimento de medicamentos a clientes, afetando negativamente sua reputação e ações na bolsa.</t>
+  </si>
 </sst>
 </file>
 
@@ -5077,7 +5437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5085,6 +5445,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5387,10 +5748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA121"/>
+  <dimension ref="A1:AA129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:S121"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123:XFD129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11589,7 +11950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>775</v>
       </c>
@@ -11636,7 +11997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>780</v>
       </c>
@@ -11683,7 +12044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>785</v>
       </c>
@@ -11730,7 +12091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>790</v>
       </c>
@@ -11777,7 +12138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>795</v>
       </c>
@@ -11824,7 +12185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>800</v>
       </c>
@@ -11871,7 +12232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>805</v>
       </c>
@@ -11918,7 +12279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>810</v>
       </c>
@@ -11965,7 +12326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>815</v>
       </c>
@@ -12010,6 +12371,490 @@
       </c>
       <c r="S121">
         <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>820</v>
+      </c>
+      <c r="B122" s="5">
+        <v>45275</v>
+      </c>
+      <c r="C122" t="s">
+        <v>821</v>
+      </c>
+      <c r="D122" t="s">
+        <v>822</v>
+      </c>
+      <c r="E122" t="s">
+        <v>823</v>
+      </c>
+      <c r="F122" t="s">
+        <v>824</v>
+      </c>
+      <c r="G122" t="s">
+        <v>825</v>
+      </c>
+      <c r="H122" t="s">
+        <v>826</v>
+      </c>
+      <c r="I122" t="s">
+        <v>827</v>
+      </c>
+      <c r="K122" t="s">
+        <v>828</v>
+      </c>
+      <c r="O122" t="s">
+        <v>28</v>
+      </c>
+      <c r="P122" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>829</v>
+      </c>
+      <c r="R122" t="s">
+        <v>830</v>
+      </c>
+      <c r="S122">
+        <v>1</v>
+      </c>
+      <c r="T122" t="s">
+        <v>831</v>
+      </c>
+      <c r="U122" t="s">
+        <v>29</v>
+      </c>
+      <c r="V122" t="s">
+        <v>28</v>
+      </c>
+      <c r="W122">
+        <v>1</v>
+      </c>
+      <c r="X122" t="s">
+        <v>832</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>833</v>
+      </c>
+      <c r="AA122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>834</v>
+      </c>
+      <c r="B123" s="5">
+        <v>44594</v>
+      </c>
+      <c r="C123" t="s">
+        <v>835</v>
+      </c>
+      <c r="D123" t="s">
+        <v>836</v>
+      </c>
+      <c r="E123" t="s">
+        <v>837</v>
+      </c>
+      <c r="K123" t="s">
+        <v>838</v>
+      </c>
+      <c r="O123" t="s">
+        <v>28</v>
+      </c>
+      <c r="P123" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>839</v>
+      </c>
+      <c r="R123" t="s">
+        <v>840</v>
+      </c>
+      <c r="S123">
+        <v>1</v>
+      </c>
+      <c r="T123" t="s">
+        <v>841</v>
+      </c>
+      <c r="U123" t="s">
+        <v>29</v>
+      </c>
+      <c r="V123" t="s">
+        <v>28</v>
+      </c>
+      <c r="W123">
+        <v>0.3</v>
+      </c>
+      <c r="X123" t="s">
+        <v>842</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z123" t="s">
+        <v>843</v>
+      </c>
+      <c r="AA123">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>844</v>
+      </c>
+      <c r="B124" s="5">
+        <v>44868</v>
+      </c>
+      <c r="C124" t="s">
+        <v>845</v>
+      </c>
+      <c r="D124" t="s">
+        <v>846</v>
+      </c>
+      <c r="E124" t="s">
+        <v>837</v>
+      </c>
+      <c r="K124" t="s">
+        <v>847</v>
+      </c>
+      <c r="O124" t="s">
+        <v>139</v>
+      </c>
+      <c r="P124" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>848</v>
+      </c>
+      <c r="R124" t="s">
+        <v>849</v>
+      </c>
+      <c r="S124">
+        <v>1</v>
+      </c>
+      <c r="T124" t="s">
+        <v>850</v>
+      </c>
+      <c r="U124" t="s">
+        <v>29</v>
+      </c>
+      <c r="V124" t="s">
+        <v>139</v>
+      </c>
+      <c r="W124">
+        <v>0.9</v>
+      </c>
+      <c r="X124" t="s">
+        <v>851</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>852</v>
+      </c>
+      <c r="AA124">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>853</v>
+      </c>
+      <c r="B125" s="5">
+        <v>44886</v>
+      </c>
+      <c r="C125" t="s">
+        <v>854</v>
+      </c>
+      <c r="D125" t="s">
+        <v>156</v>
+      </c>
+      <c r="E125" t="s">
+        <v>837</v>
+      </c>
+      <c r="K125" t="s">
+        <v>855</v>
+      </c>
+      <c r="O125" t="s">
+        <v>139</v>
+      </c>
+      <c r="P125" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>856</v>
+      </c>
+      <c r="R125" t="s">
+        <v>857</v>
+      </c>
+      <c r="S125">
+        <v>1</v>
+      </c>
+      <c r="T125" t="s">
+        <v>858</v>
+      </c>
+      <c r="U125" t="s">
+        <v>29</v>
+      </c>
+      <c r="V125" t="s">
+        <v>139</v>
+      </c>
+      <c r="W125">
+        <v>0.8</v>
+      </c>
+      <c r="X125" t="s">
+        <v>851</v>
+      </c>
+      <c r="Y125" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>859</v>
+      </c>
+      <c r="AA125">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>860</v>
+      </c>
+      <c r="B126" s="5">
+        <v>44893</v>
+      </c>
+      <c r="C126" t="s">
+        <v>861</v>
+      </c>
+      <c r="D126" t="s">
+        <v>862</v>
+      </c>
+      <c r="E126" t="s">
+        <v>837</v>
+      </c>
+      <c r="K126" t="s">
+        <v>863</v>
+      </c>
+      <c r="O126" t="s">
+        <v>33</v>
+      </c>
+      <c r="P126" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>864</v>
+      </c>
+      <c r="R126" t="s">
+        <v>865</v>
+      </c>
+      <c r="S126">
+        <v>1</v>
+      </c>
+      <c r="T126" t="s">
+        <v>866</v>
+      </c>
+      <c r="U126" t="s">
+        <v>29</v>
+      </c>
+      <c r="V126" t="s">
+        <v>33</v>
+      </c>
+      <c r="W126">
+        <v>0.8</v>
+      </c>
+      <c r="X126" t="s">
+        <v>867</v>
+      </c>
+      <c r="Y126" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>868</v>
+      </c>
+      <c r="AA126">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>869</v>
+      </c>
+      <c r="B127" s="5">
+        <v>44897</v>
+      </c>
+      <c r="C127" t="s">
+        <v>870</v>
+      </c>
+      <c r="D127" t="s">
+        <v>871</v>
+      </c>
+      <c r="E127" t="s">
+        <v>837</v>
+      </c>
+      <c r="K127" t="s">
+        <v>872</v>
+      </c>
+      <c r="O127" t="s">
+        <v>28</v>
+      </c>
+      <c r="P127" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>873</v>
+      </c>
+      <c r="R127" t="s">
+        <v>874</v>
+      </c>
+      <c r="S127">
+        <v>1</v>
+      </c>
+      <c r="T127" t="s">
+        <v>875</v>
+      </c>
+      <c r="U127" t="s">
+        <v>29</v>
+      </c>
+      <c r="V127" t="s">
+        <v>28</v>
+      </c>
+      <c r="W127">
+        <v>-0.2</v>
+      </c>
+      <c r="X127" t="s">
+        <v>876</v>
+      </c>
+      <c r="Y127" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z127" t="s">
+        <v>877</v>
+      </c>
+      <c r="AA127">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>878</v>
+      </c>
+      <c r="B128" s="5">
+        <v>45251</v>
+      </c>
+      <c r="C128" t="s">
+        <v>879</v>
+      </c>
+      <c r="D128" t="s">
+        <v>880</v>
+      </c>
+      <c r="E128" t="s">
+        <v>837</v>
+      </c>
+      <c r="K128" t="s">
+        <v>881</v>
+      </c>
+      <c r="O128" t="s">
+        <v>139</v>
+      </c>
+      <c r="P128" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>882</v>
+      </c>
+      <c r="R128" t="s">
+        <v>883</v>
+      </c>
+      <c r="S128">
+        <v>1</v>
+      </c>
+      <c r="T128" t="s">
+        <v>884</v>
+      </c>
+      <c r="U128" t="s">
+        <v>29</v>
+      </c>
+      <c r="V128" t="s">
+        <v>139</v>
+      </c>
+      <c r="W128">
+        <v>1</v>
+      </c>
+      <c r="X128" t="s">
+        <v>851</v>
+      </c>
+      <c r="Y128" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z128" t="s">
+        <v>885</v>
+      </c>
+      <c r="AA128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>886</v>
+      </c>
+      <c r="B129" s="5">
+        <v>45314</v>
+      </c>
+      <c r="C129" t="s">
+        <v>887</v>
+      </c>
+      <c r="D129" t="s">
+        <v>156</v>
+      </c>
+      <c r="E129" t="s">
+        <v>837</v>
+      </c>
+      <c r="K129" t="s">
+        <v>888</v>
+      </c>
+      <c r="O129" t="s">
+        <v>139</v>
+      </c>
+      <c r="P129" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>889</v>
+      </c>
+      <c r="R129" t="s">
+        <v>890</v>
+      </c>
+      <c r="S129">
+        <v>1</v>
+      </c>
+      <c r="T129" t="s">
+        <v>891</v>
+      </c>
+      <c r="U129" t="s">
+        <v>29</v>
+      </c>
+      <c r="V129" t="s">
+        <v>139</v>
+      </c>
+      <c r="W129">
+        <v>-0.8</v>
+      </c>
+      <c r="X129" t="s">
+        <v>892</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z129" t="s">
+        <v>893</v>
+      </c>
+      <c r="AA129">
+        <v>-0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>